<commit_message>
Linear regresi 8 April 2020
</commit_message>
<xml_diff>
--- a/calculate.xlsx
+++ b/calculate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Linear Regresi</t>
   </si>
@@ -50,9 +50,6 @@
     <t>b / m / gradien /slope /kemiringan</t>
   </si>
   <si>
-    <t>y_bestline</t>
-  </si>
-  <si>
     <t>max error |y-y'|</t>
   </si>
   <si>
@@ -75,6 +72,48 @@
   </si>
   <si>
     <t>MSE</t>
+  </si>
+  <si>
+    <t>Root Mean Squared Error</t>
+  </si>
+  <si>
+    <t>MedAE (Median Absolute Error)</t>
+  </si>
+  <si>
+    <t>MSLE (Mean Squared Algoritmic Error)</t>
+  </si>
+  <si>
+    <t>elog(1+y)</t>
+  </si>
+  <si>
+    <t>elog(1+y')</t>
+  </si>
+  <si>
+    <t>y_bestline / prediction</t>
+  </si>
+  <si>
+    <t>(elog(1+y)-elog(1+y'))^2</t>
+  </si>
+  <si>
+    <t>RMSLE</t>
+  </si>
+  <si>
+    <t>R^2 Score</t>
+  </si>
+  <si>
+    <t>|y-avgy|</t>
+  </si>
+  <si>
+    <t>|y-avgy|^2</t>
+  </si>
+  <si>
+    <t>SUM error</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
@@ -83,7 +122,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -124,7 +163,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -270,6 +309,94 @@
         <a:xfrm>
           <a:off x="6887308" y="3634155"/>
           <a:ext cx="1611923" cy="444668"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10264</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>8277</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1747161</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>149081</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6876547" y="4580277"/>
+          <a:ext cx="1736897" cy="521804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2443369</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>120204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6866283" y="5905500"/>
+          <a:ext cx="2443369" cy="501204"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -544,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,22 +682,25 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -584,19 +714,34 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -627,8 +772,28 @@
         <f>ABS(E6-B6)^2</f>
         <v>10.240000000000064</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>B6-(AVERAGE($B$6:$B$11))</f>
+        <v>-58</v>
+      </c>
+      <c r="K6">
+        <f>J6^2</f>
+        <v>3364</v>
+      </c>
+      <c r="L6">
+        <f>LN(1+B6)</f>
+        <v>2.3978952727983707</v>
+      </c>
+      <c r="M6">
+        <f>LN(1+E6)</f>
+        <v>2.0541237336955449</v>
+      </c>
+      <c r="N6">
+        <f>(L6-M6)^2</f>
+        <v>0.11817887109712566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -636,15 +801,15 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C11" si="0">A7^2</f>
+        <f t="shared" ref="C7:C10" si="0">A7^2</f>
         <v>4000000</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D11" si="1">A7*B7</f>
+        <f t="shared" ref="D7:D10" si="1">A7*B7</f>
         <v>50000</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E11" si="2">(A7*$C$18)+($C$15)</f>
+        <f t="shared" ref="E7:E10" si="2">(A7*$C$18)+($C$15)</f>
         <v>23.79999999999999</v>
       </c>
       <c r="G7">
@@ -659,8 +824,28 @@
         <f t="shared" ref="I7:I10" si="5">ABS(E7-B7)^2</f>
         <v>1.4400000000000239</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" ref="J7:J10" si="6">B7-(AVERAGE($B$6:$B$11))</f>
+        <v>-43</v>
+      </c>
+      <c r="K7">
+        <f>J7^2</f>
+        <v>1849</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L10" si="7">LN(1+B7)</f>
+        <v>3.2580965380214821</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M10" si="8">LN(1+E7)</f>
+        <v>3.2108436531709361</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N10" si="9">(L7-M7)^2</f>
+        <v>2.2328351266989615E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3000</v>
       </c>
@@ -691,8 +876,28 @@
         <f t="shared" si="5"/>
         <v>46.239999999999959</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>-34</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K7:K10" si="10">J8^2</f>
+        <v>1156</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>3.5553480614894135</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>3.7328963395307104</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="9"/>
+        <v>3.1523391035429678E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4000</v>
       </c>
@@ -723,8 +928,28 @@
         <f t="shared" si="5"/>
         <v>7.8399999999999439</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>-13</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="10"/>
+        <v>169</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="7"/>
+        <v>4.0253516907351496</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>4.0741418549045809</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="9"/>
+        <v>2.3804801196800553E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5000</v>
       </c>
@@ -755,22 +980,42 @@
         <f t="shared" si="5"/>
         <v>27.040000000000177</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>4.3944491546724391</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
+        <v>4.3280982926483258</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="9"/>
+        <v>4.4024368913429248E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>SUM(A6:A10)</f>
         <v>15000</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:D11" si="6">SUM(B6:B10)</f>
+        <f t="shared" ref="B11:D11" si="11">SUM(B6:B10)</f>
         <v>204</v>
       </c>
       <c r="C11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>55000000</v>
       </c>
       <c r="D11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>782000</v>
       </c>
       <c r="H11" s="2">
@@ -781,16 +1026,30 @@
         <f>SUM(I6:I10)/5</f>
         <v>18.560000000000034</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f>SUM(K6:K10)</f>
+        <v>6682</v>
+      </c>
+      <c r="N11">
+        <f>SUM(N6:N10)</f>
+        <v>0.15871801427027729</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>SUM(I6:I10)</f>
+        <v>92.800000000000168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -799,31 +1058,67 @@
         <v>-10.199999999999999</v>
       </c>
       <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
         <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
       </c>
       <c r="G14">
         <v>6.8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>INTERCEPT(B6:B10,A6:A10)</f>
         <v>-10.20000000000001</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <f>H11</f>
+        <v>3.8400000000000047</v>
+      </c>
+      <c r="U15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
         <v>10</v>
       </c>
-      <c r="G15">
-        <v>3.84</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>4</v>
+      </c>
+      <c r="R16">
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <f>ABS(-6)</f>
+        <v>6</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="U16">
+        <f>SUM(P16:T16)</f>
+        <v>22</v>
+      </c>
+      <c r="V16">
+        <f>U16/5</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -832,21 +1127,184 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>SLOPE(B6:B10,A6:A10)</f>
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18">
+        <f>3^2</f>
+        <v>9</v>
+      </c>
+      <c r="Q18">
+        <f>Q16^2</f>
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <f>R16^2</f>
+        <v>25</v>
+      </c>
+      <c r="S18">
+        <f>-6^2</f>
+        <v>36</v>
+      </c>
+      <c r="T18">
+        <f>T16^2</f>
+        <v>16</v>
+      </c>
+      <c r="U18">
+        <f>SUM(P18:T18)</f>
+        <v>102</v>
+      </c>
+      <c r="V18">
+        <f>U18/5</f>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <f>I11</f>
+        <v>18.560000000000034</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>29</v>
+      </c>
+      <c r="V20">
+        <f>SQRT(V18)</f>
+        <v>4.5166359162544856</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>2</v>
+      </c>
+      <c r="U23">
+        <f>SUM(P23:T23)</f>
+        <v>10</v>
+      </c>
+      <c r="V23">
+        <f>U23/5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <f>SQRT(G19)</f>
+        <v>4.3081318457076074</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
         <v>15</v>
       </c>
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <v>18.559999999999999</v>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>4</v>
+      </c>
+      <c r="R25">
+        <v>4</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <v>4</v>
+      </c>
+      <c r="U25">
+        <f>SUM(P25:T25)</f>
+        <v>20</v>
+      </c>
+      <c r="V25">
+        <f>U25/5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>29</v>
+      </c>
+      <c r="V27">
+        <f>SQRT(V25)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29">
+        <f>MEDIAN(G6:G10)</f>
+        <v>3.2000000000000099</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <f>N11/5</f>
+        <v>3.1743602854055461E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35">
+        <f>SQRT(G31)</f>
+        <v>0.17816734508336668</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <f>1-(I12/K11)</f>
+        <v>0.98611194253217593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>